<commit_message>
Update on 20200416 part 2
</commit_message>
<xml_diff>
--- a/文档/测试工作相关/IT端到端测试相关/测试内容相关/2020/20200416/增加停机用户资源释放后，复机时支持新装光的流程(196215088)/增加停机用户资源释放后，复机时支持新装光的流程（196215088 ）测试结果.xlsx
+++ b/文档/测试工作相关/IT端到端测试相关/测试内容相关/2020/20200416/增加停机用户资源释放后，复机时支持新装光的流程(196215088)/增加停机用户资源释放后，复机时支持新装光的流程（196215088 ）测试结果.xlsx
@@ -154,11 +154,11 @@
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>WMX2020041505328048</t>
+    <t>IBP域</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>IBP域</t>
+    <t>WMX2020041605329388</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -617,7 +617,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.25" defaultRowHeight="13.5"/>
   <cols>
@@ -946,7 +948,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="20" t="s">
@@ -956,7 +958,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I2" s="22" t="s">
         <v>28</v>

</xml_diff>